<commit_message>
ferdig med excel dokumenter trakt
</commit_message>
<xml_diff>
--- a/Resultater/excel-plot/630Ad6.0.xlsx
+++ b/Resultater/excel-plot/630Ad6.0.xlsx
@@ -4,23 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="360" windowWidth="28275" windowHeight="12315" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="360" windowWidth="28275" windowHeight="12315" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="630Adata" sheetId="1" r:id="rId1"/>
     <sheet name="graf" sheetId="2" r:id="rId2"/>
     <sheet name="880Adata" sheetId="3" r:id="rId3"/>
     <sheet name="geoB630A" sheetId="4" r:id="rId4"/>
+    <sheet name="geoB880A" sheetId="5" r:id="rId5"/>
+    <sheet name="comp" sheetId="6" r:id="rId6"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
   <si>
     <t>Pressure</t>
   </si>
@@ -59,6 +58,27 @@
   </si>
   <si>
     <t>880 A</t>
+  </si>
+  <si>
+    <t>880A</t>
+  </si>
+  <si>
+    <t>Succsesrate funnel</t>
+  </si>
+  <si>
+    <t>pressure</t>
+  </si>
+  <si>
+    <t>A,630</t>
+  </si>
+  <si>
+    <t>A,880</t>
+  </si>
+  <si>
+    <t>B,630</t>
+  </si>
+  <si>
+    <t>B,880</t>
   </si>
 </sst>
 </file>
@@ -181,7 +201,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>630 A</c:v>
+            <c:v>630 A Geometry a</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="63500">
@@ -243,11 +263,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="103616896"/>
-        <c:axId val="103800192"/>
+        <c:axId val="86800256"/>
+        <c:axId val="86823680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103616896"/>
+        <c:axId val="86800256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -284,14 +304,14 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103800192"/>
+        <c:crossAx val="86823680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103800192"/>
+        <c:axId val="86823680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -336,7 +356,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103616896"/>
+        <c:crossAx val="86800256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -347,10 +367,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.72810767619564809"/>
+          <c:x val="0.7281076761956482"/>
           <c:y val="0.30778953759129896"/>
-          <c:w val="0.18877633399273369"/>
-          <c:h val="0.11675207030714954"/>
+          <c:w val="0.24788963448534451"/>
+          <c:h val="0.11675207030714956"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -396,7 +416,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>630 A Inside funnle</c:v>
+            <c:v>630 A Inside funnel</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="63500">
@@ -525,11 +545,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="103796736"/>
-        <c:axId val="103854464"/>
+        <c:axId val="86979328"/>
+        <c:axId val="86981632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103796736"/>
+        <c:axId val="86979328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -566,14 +586,14 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103854464"/>
+        <c:crossAx val="86981632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103854464"/>
+        <c:axId val="86981632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -618,7 +638,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103796736"/>
+        <c:crossAx val="86979328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -632,7 +652,7 @@
           <c:x val="0.69001243810040991"/>
           <c:y val="0.31719245249491912"/>
           <c:w val="0.26663780820500893"/>
-          <c:h val="0.14622509985969667"/>
+          <c:h val="0.14622509985969673"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -678,7 +698,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>880 A</c:v>
+            <c:v>880 A Geometry a</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="127000">
@@ -689,7 +709,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="20"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="9BBB59"/>
@@ -740,11 +760,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="87931904"/>
-        <c:axId val="87934848"/>
+        <c:axId val="86776448"/>
+        <c:axId val="87012480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87931904"/>
+        <c:axId val="86776448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -781,14 +801,14 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87934848"/>
+        <c:crossAx val="87012480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87934848"/>
+        <c:axId val="87012480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -833,7 +853,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87931904"/>
+        <c:crossAx val="86776448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -844,10 +864,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.72810767619564831"/>
-          <c:y val="0.30778953759129896"/>
-          <c:w val="0.1887763339927338"/>
-          <c:h val="0.11675207030714957"/>
+          <c:x val="0.73073493399531964"/>
+          <c:y val="0.30402837162985091"/>
+          <c:w val="0.24394874778583711"/>
+          <c:h val="0.11675207030714958"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -893,7 +913,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>630 A</c:v>
+            <c:v>630 A Geometry b</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="63500">
@@ -904,7 +924,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="10"/>
+            <c:size val="20"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -955,11 +975,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="103912576"/>
-        <c:axId val="106963328"/>
+        <c:axId val="87036672"/>
+        <c:axId val="87038976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103912576"/>
+        <c:axId val="87036672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -996,14 +1016,14 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106963328"/>
+        <c:crossAx val="87038976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106963328"/>
+        <c:axId val="87038976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1048,7 +1068,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103912576"/>
+        <c:crossAx val="87036672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1059,10 +1079,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.72810767619564853"/>
+          <c:x val="0.71891227389679746"/>
           <c:y val="0.30778953759129896"/>
-          <c:w val="0.18877633399273391"/>
-          <c:h val="0.1167520703071496"/>
+          <c:w val="0.23738060328665814"/>
+          <c:h val="0.11675207030714961"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -1108,7 +1128,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>630 A Inside funnle</c:v>
+            <c:v>630 A Inside funnel</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="63500">
@@ -1122,7 +1142,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="10"/>
+            <c:size val="20"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent4">
@@ -1186,7 +1206,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="square"/>
-            <c:size val="10"/>
+            <c:size val="20"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="C00000"/>
@@ -1237,11 +1257,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="102601856"/>
-        <c:axId val="102864768"/>
+        <c:axId val="87067648"/>
+        <c:axId val="87090688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102601856"/>
+        <c:axId val="87067648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1278,14 +1298,14 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="102864768"/>
+        <c:crossAx val="87090688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102864768"/>
+        <c:axId val="87090688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1330,7 +1350,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="102601856"/>
+        <c:crossAx val="87067648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1344,7 +1364,888 @@
           <c:x val="0.69001243810040991"/>
           <c:y val="0.31719245249491912"/>
           <c:w val="0.26663780820500893"/>
-          <c:h val="0.14622509985969676"/>
+          <c:h val="0.14622509985969678"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800"/>
+          </a:pPr>
+          <a:endParaRPr lang="nb-NO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln w="9525"/>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="nb-NO"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>880 A Geometry b</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="127000">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="20"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>geoB880A!$G$5:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>geoB880A!$I$5:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="85019264"/>
+        <c:axId val="85066880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="85019264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO" sz="1800"/>
+                  <a:t>Upstream over-pressure [bar]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="85066880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="85066880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO" sz="1800"/>
+                  <a:t>Successful interruptions [%]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="85019264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.71891227389679768"/>
+          <c:y val="0.30778953759129896"/>
+          <c:w val="0.23738060328665808"/>
+          <c:h val="0.11675207030714962"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800"/>
+          </a:pPr>
+          <a:endParaRPr lang="nb-NO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln w="9525"/>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="nb-NO"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>880 A Inside funnel</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="127000">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="20"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>geoB880A!$G$5:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>geoB880A!$L$5:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>880 A Outside nozzle</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="127000"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="20"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>geoB880A!$G$5:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>geoB880A!$N$5:$N$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="87108224"/>
+        <c:axId val="87121280"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="87108224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO" sz="1800"/>
+                  <a:t>Upstream over-pressure [bar]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="87121280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="87121280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO" sz="1800"/>
+                  <a:t>Successful interruptions [%]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="87108224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.69001243810040991"/>
+          <c:y val="0.31719245249491912"/>
+          <c:w val="0.26663780820500893"/>
+          <c:h val="0.14622509985969684"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800"/>
+          </a:pPr>
+          <a:endParaRPr lang="nb-NO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln w="9525"/>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="nb-NO"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>630 A Geometry a</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="63500">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="9BBB59"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>comp!$B$3:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>comp!$C$3:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>880 A Geometry a</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="127000">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>comp!$D$3:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>630 A Geometry b</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="63500">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="20"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>comp!$E$3:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>880 A Geometry b</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="127000">
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="20"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="4F81BD"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>comp!$F$3:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="109791104"/>
+        <c:axId val="109802624"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="109791104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO" sz="1800"/>
+                  <a:t>Upstream over-pressure [bar]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="109802624"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="109802624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO" sz="1800"/>
+                  <a:t>Successful interruptions [%]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="109791104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.72022590279663323"/>
+          <c:y val="0.17426814595989323"/>
+          <c:w val="0.27189232380435202"/>
+          <c:h val="0.47908828744784898"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -1483,14 +2384,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1542,119 +2443,104 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Ark1"/>
-      <sheetName val="Ark2"/>
-      <sheetName val="Ark3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="I3" t="str">
-            <v>Test less than 35 are dicarded due to transcation effects from the nozzle</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="I4" t="str">
-            <v>630 A</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="H5" t="str">
-            <v>Pressure</v>
-          </cell>
-          <cell r="I5" t="str">
-            <v>Amount of successful</v>
-          </cell>
-          <cell r="J5" t="str">
-            <v>Successrate</v>
-          </cell>
-          <cell r="K5" t="str">
-            <v>Number of tests</v>
-          </cell>
-          <cell r="L5" t="str">
-            <v>Total Succsessrate</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="H6">
-            <v>0.2</v>
-          </cell>
-          <cell r="I6">
-            <v>0</v>
-          </cell>
-          <cell r="J6">
-            <v>0</v>
-          </cell>
-          <cell r="K6">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="H7">
-            <v>0.25</v>
-          </cell>
-          <cell r="I7">
-            <v>0</v>
-          </cell>
-          <cell r="J7">
-            <v>0</v>
-          </cell>
-          <cell r="K7">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="H8">
-            <v>0.3</v>
-          </cell>
-          <cell r="I8">
-            <v>8</v>
-          </cell>
-          <cell r="J8">
-            <v>80</v>
-          </cell>
-          <cell r="K8">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="H9">
-            <v>0.35</v>
-          </cell>
-          <cell r="I9">
-            <v>4</v>
-          </cell>
-          <cell r="J9">
-            <v>80</v>
-          </cell>
-          <cell r="K9">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="H10">
-            <v>0.4</v>
-          </cell>
-          <cell r="I10">
-            <v>5</v>
-          </cell>
-          <cell r="J10">
-            <v>100</v>
-          </cell>
-          <cell r="K10">
-            <v>5</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagram 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagram 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>638174</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>628649</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagram 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1944,8 +2830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:N10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2117,7 +3003,7 @@
         <v>6</v>
       </c>
       <c r="I8" s="6">
-        <f t="shared" ref="I7:I11" si="0">H8/J8*100</f>
+        <f t="shared" ref="I8:I10" si="0">H8/J8*100</f>
         <v>60</v>
       </c>
       <c r="J8">
@@ -2667,8 +3553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2683,7 +3569,7 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U33" sqref="U33"/>
+      <selection activeCell="I5" sqref="I5:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3351,8 +4237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4016,4 +4902,953 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N66"/>
+  <sheetViews>
+    <sheetView topLeftCell="M10" workbookViewId="0">
+      <selection activeCell="T45" sqref="T45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="12" max="12" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A3" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>35</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0.25</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <f>H5/J5*100</f>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <f>K5/5*100</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <f>M5/5*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0.3</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6" s="6">
+        <f t="shared" ref="I6:I8" si="0">H6/J6*100</f>
+        <v>80</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6" s="6">
+        <f>K6/5*100</f>
+        <v>60</v>
+      </c>
+      <c r="M6" s="4">
+        <v>5</v>
+      </c>
+      <c r="N6" s="6">
+        <f t="shared" ref="N6:N8" si="1">M6/5*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="B7" s="4">
+        <v>46</v>
+      </c>
+      <c r="C7" s="2">
+        <v>101</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0.35</v>
+      </c>
+      <c r="H7">
+        <v>9</v>
+      </c>
+      <c r="I7" s="6">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7" s="6">
+        <f t="shared" ref="L7:L8" si="2">K7/5*100</f>
+        <v>80</v>
+      </c>
+      <c r="M7" s="4">
+        <v>4</v>
+      </c>
+      <c r="N7" s="6">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A8" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="B8" s="4">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0.4</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8" s="7">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8" s="7">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="M8" s="4">
+        <v>4</v>
+      </c>
+      <c r="N8" s="7">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="B9" s="4">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="B10" s="4">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="B12" s="2">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2">
+        <v>70</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="B13" s="2">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="B14" s="2">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="B15" s="4">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="B16" s="4">
+        <v>32</v>
+      </c>
+      <c r="C16" s="2">
+        <v>83</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="B17" s="4">
+        <v>13</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="B18" s="4">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="B19" s="4">
+        <v>12</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="B20" s="4">
+        <v>13</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="B21" s="1">
+        <v>35</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="B22" s="2">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="B23" s="2">
+        <v>17</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="B24" s="2">
+        <v>17</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="B25" s="4">
+        <v>25</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="B26" s="4">
+        <v>28</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="B27" s="4">
+        <v>32</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="B28" s="4">
+        <v>35</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="B29" s="4">
+        <v>16</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="B30" s="4">
+        <v>17</v>
+      </c>
+      <c r="C30" s="2">
+        <v>74</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="B31" s="1">
+        <v>14</v>
+      </c>
+      <c r="C31" s="1">
+        <v>71</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="B32" s="3">
+        <v>11</v>
+      </c>
+      <c r="C32" s="3">
+        <v>66</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="B33" s="4">
+        <v>23</v>
+      </c>
+      <c r="C33" s="4">
+        <v>77</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="B34" s="4">
+        <v>29</v>
+      </c>
+      <c r="C34" s="4">
+        <v>84</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="B35" s="4">
+        <v>22</v>
+      </c>
+      <c r="C35" s="4">
+        <v>78</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="B36" s="4">
+        <v>37</v>
+      </c>
+      <c r="C36" s="4">
+        <v>91</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="B37" s="4">
+        <v>18</v>
+      </c>
+      <c r="C37" s="4">
+        <v>72</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="B38" s="4">
+        <v>16</v>
+      </c>
+      <c r="C38" s="4">
+        <v>72</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="B39" s="4">
+        <v>12</v>
+      </c>
+      <c r="C39" s="4">
+        <v>66</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="B40" s="4">
+        <v>15</v>
+      </c>
+      <c r="C40" s="4">
+        <v>69</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="B41" s="1">
+        <v>34</v>
+      </c>
+      <c r="C41" s="1">
+        <v>88</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="2"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="2"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="2"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="2"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="2"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="2"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="2"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="2"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="2"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="2"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="2"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="2"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="2"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="2"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="2"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="2"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3">
+        <v>0.15</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>60</v>
+      </c>
+      <c r="E4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5">
+        <v>0.25</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <v>90</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6">
+        <v>0.3</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7">
+        <v>0.35</v>
+      </c>
+      <c r="F7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8">
+        <v>0.4</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9">
+        <v>0.5</v>
+      </c>
+      <c r="D9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10">
+        <v>0.6</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
oppdatert resultater etter feil i geo a 630 A test
</commit_message>
<xml_diff>
--- a/Resultater/excel-plot/630Ad6.0.xlsx
+++ b/Resultater/excel-plot/630Ad6.0.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="25">
   <si>
     <t>Pressure</t>
   </si>
@@ -79,6 +79,21 @@
   </si>
   <si>
     <t>B,880</t>
+  </si>
+  <si>
+    <t>20+</t>
+  </si>
+  <si>
+    <t>geoA630</t>
+  </si>
+  <si>
+    <t>success rate=</t>
+  </si>
+  <si>
+    <t>10+</t>
+  </si>
+  <si>
+    <t>antall: 18</t>
   </si>
 </sst>
 </file>
@@ -253,7 +268,7 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>100</c:v>
@@ -263,11 +278,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="117696384"/>
-        <c:axId val="117703040"/>
+        <c:axId val="59144832"/>
+        <c:axId val="59163776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="117696384"/>
+        <c:axId val="59144832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -304,14 +319,14 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117703040"/>
+        <c:crossAx val="59163776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117703040"/>
+        <c:axId val="59163776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -356,7 +371,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117696384"/>
+        <c:crossAx val="59144832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -367,10 +382,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.72810767619564831"/>
+          <c:x val="0.72810767619564842"/>
           <c:y val="0.30778953759129896"/>
-          <c:w val="0.24788963448534454"/>
-          <c:h val="0.11675207030714957"/>
+          <c:w val="0.24788963448534457"/>
+          <c:h val="0.11675207030714958"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -545,11 +560,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="117723520"/>
-        <c:axId val="117725824"/>
+        <c:axId val="59290752"/>
+        <c:axId val="59293056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="117723520"/>
+        <c:axId val="59290752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -586,14 +601,14 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117725824"/>
+        <c:crossAx val="59293056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117725824"/>
+        <c:axId val="59293056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -638,7 +653,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117723520"/>
+        <c:crossAx val="59290752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -652,7 +667,7 @@
           <c:x val="0.69001243810040991"/>
           <c:y val="0.31719245249491912"/>
           <c:w val="0.26663780820500893"/>
-          <c:h val="0.14622509985969676"/>
+          <c:h val="0.14622509985969678"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -760,11 +775,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="117926144"/>
-        <c:axId val="117936896"/>
+        <c:axId val="59230848"/>
+        <c:axId val="59237504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="117926144"/>
+        <c:axId val="59230848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -786,6 +801,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -800,14 +816,14 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117936896"/>
+        <c:crossAx val="59237504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117936896"/>
+        <c:axId val="59237504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -830,6 +846,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -851,7 +868,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117926144"/>
+        <c:crossAx val="59230848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -863,9 +880,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.73073493399531964"/>
-          <c:y val="0.30402837162985108"/>
-          <c:w val="0.24394874778583717"/>
-          <c:h val="0.1167520703071496"/>
+          <c:y val="0.30402837162985125"/>
+          <c:w val="0.24394874778583725"/>
+          <c:h val="0.11675207030714961"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -973,11 +990,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="117854592"/>
-        <c:axId val="117856896"/>
+        <c:axId val="59343616"/>
+        <c:axId val="59345920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="117854592"/>
+        <c:axId val="59343616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -999,6 +1016,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1013,14 +1031,14 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117856896"/>
+        <c:crossAx val="59345920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117856896"/>
+        <c:axId val="59345920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1043,6 +1061,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1064,7 +1083,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117854592"/>
+        <c:crossAx val="59343616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1075,9 +1094,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.71891227389679757"/>
+          <c:x val="0.71891227389679768"/>
           <c:y val="0.30778953759129896"/>
-          <c:w val="0.23738060328665811"/>
+          <c:w val="0.23738060328665808"/>
           <c:h val="0.11675207030714962"/>
         </c:manualLayout>
       </c:layout>
@@ -1253,11 +1272,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="117881088"/>
-        <c:axId val="117965568"/>
+        <c:axId val="59358208"/>
+        <c:axId val="59454976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="117881088"/>
+        <c:axId val="59358208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1279,6 +1298,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1293,14 +1313,14 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117965568"/>
+        <c:crossAx val="59454976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117965568"/>
+        <c:axId val="59454976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1323,6 +1343,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1344,7 +1365,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117881088"/>
+        <c:crossAx val="59358208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1358,7 +1379,7 @@
           <c:x val="0.69001243810040991"/>
           <c:y val="0.31719245249491912"/>
           <c:w val="0.26663780820500893"/>
-          <c:h val="0.14622509985969681"/>
+          <c:h val="0.14622509985969684"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -1466,11 +1487,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="118038912"/>
-        <c:axId val="118041216"/>
+        <c:axId val="59516032"/>
+        <c:axId val="59518336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="118038912"/>
+        <c:axId val="59516032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1492,6 +1513,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1506,14 +1528,14 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118041216"/>
+        <c:crossAx val="59518336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118041216"/>
+        <c:axId val="59518336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1536,6 +1558,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1557,7 +1580,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118038912"/>
+        <c:crossAx val="59516032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1570,7 +1593,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.71891227389679768"/>
           <c:y val="0.30778953759129896"/>
-          <c:w val="0.23738060328665805"/>
+          <c:w val="0.23738060328665803"/>
           <c:h val="0.11675207030714962"/>
         </c:manualLayout>
       </c:layout>
@@ -1751,11 +1774,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="118065792"/>
-        <c:axId val="118084736"/>
+        <c:axId val="59551104"/>
+        <c:axId val="62068608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="118065792"/>
+        <c:axId val="59551104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1777,6 +1800,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1791,14 +1815,14 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118084736"/>
+        <c:crossAx val="62068608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118084736"/>
+        <c:axId val="62068608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1821,6 +1845,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1842,7 +1867,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118065792"/>
+        <c:crossAx val="59551104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1856,7 +1881,7 @@
           <c:x val="0.69001243810040991"/>
           <c:y val="0.31719245249491912"/>
           <c:w val="0.26663780820500893"/>
-          <c:h val="0.14622509985969687"/>
+          <c:h val="0.14622509985969692"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -1971,10 +1996,10 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2128,11 +2153,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="118123520"/>
-        <c:axId val="118142464"/>
+        <c:axId val="62132224"/>
+        <c:axId val="62134528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="118123520"/>
+        <c:axId val="62132224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2169,14 +2194,14 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118142464"/>
+        <c:crossAx val="62134528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118142464"/>
+        <c:axId val="62134528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2221,7 +2246,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118123520"/>
+        <c:crossAx val="62132224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2233,9 +2258,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.72022590279663323"/>
-          <c:y val="0.17426814595989326"/>
-          <c:w val="0.27189232380435208"/>
-          <c:h val="0.47908828744784909"/>
+          <c:y val="0.17426814595989329"/>
+          <c:w val="0.27189232380435213"/>
+          <c:h val="0.47908828744784926"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -2820,8 +2845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:I10"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3029,11 +3054,11 @@
         <v>0.25</v>
       </c>
       <c r="H9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I9" s="6">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J9">
         <v>10</v>
@@ -3151,6 +3176,15 @@
       <c r="D15" s="2">
         <v>1</v>
       </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2">
@@ -3165,8 +3199,20 @@
       <c r="D16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="G16">
+        <v>0.3</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>0.3</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="2">
         <v>0.25</v>
       </c>
@@ -3177,8 +3223,20 @@
       <c r="D17" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="G17">
+        <v>0.3</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>0.3</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="2">
         <v>0.25</v>
       </c>
@@ -3189,8 +3247,20 @@
       <c r="D18" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="G18">
+        <v>0.3</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>0.3</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="2">
         <v>0.25</v>
       </c>
@@ -3201,10 +3271,22 @@
         <v>70</v>
       </c>
       <c r="D19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0.3</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0.3</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="2">
         <v>0.25</v>
       </c>
@@ -3215,8 +3297,20 @@
       <c r="D20" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="G20">
+        <v>0.3</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>0.3</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="1">
         <v>0.25</v>
       </c>
@@ -3227,8 +3321,20 @@
       <c r="D21" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="G21">
+        <v>0.3</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>0.3</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="3">
         <v>0.2</v>
       </c>
@@ -3241,8 +3347,20 @@
       <c r="D22" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="G22">
+        <v>0.3</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>0.3</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="2">
         <v>0.2</v>
       </c>
@@ -3253,8 +3371,20 @@
       <c r="D23" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="G23">
+        <v>0.3</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>0.3</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="2">
         <v>0.2</v>
       </c>
@@ -3267,8 +3397,20 @@
       <c r="D24" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="G24">
+        <v>0.3</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>0.3</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="2">
         <v>0.2</v>
       </c>
@@ -3281,8 +3423,24 @@
       <c r="D25" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="G25">
+        <v>0.3</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <f>SUM(H16:H26)</f>
+        <v>11</v>
+      </c>
+      <c r="K25">
+        <v>0.3</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="2">
         <v>0.2</v>
       </c>
@@ -3293,8 +3451,29 @@
       <c r="D26" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="G26" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26">
+        <v>100</v>
+      </c>
+      <c r="K26">
+        <v>0.3</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="2">
         <v>0.2</v>
       </c>
@@ -3305,8 +3484,20 @@
       <c r="D27" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="G27">
+        <v>0.25</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>0.3</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="2">
         <v>0.2</v>
       </c>
@@ -3317,8 +3508,20 @@
       <c r="D28" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="G28">
+        <v>0.25</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>0.3</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="2">
         <v>0.2</v>
       </c>
@@ -3331,8 +3534,20 @@
       <c r="D29" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="G29">
+        <v>0.25</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>0.3</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="2">
         <v>0.2</v>
       </c>
@@ -3343,8 +3558,20 @@
       <c r="D30" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="G30">
+        <v>0.25</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>0.3</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="1">
         <v>0.2</v>
       </c>
@@ -3356,8 +3583,20 @@
         <v>1</v>
       </c>
       <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="G31">
+        <v>0.25</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>0.3</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="3">
         <v>0.15</v>
       </c>
@@ -3371,8 +3610,20 @@
         <v>0</v>
       </c>
       <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="G32">
+        <v>0.25</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>0.3</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="2">
         <v>0.15</v>
       </c>
@@ -3386,8 +3637,24 @@
         <v>0</v>
       </c>
       <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="G33">
+        <v>0.25</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L33" s="1">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <f>100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="2">
         <v>0.15</v>
       </c>
@@ -3401,8 +3668,20 @@
         <v>0</v>
       </c>
       <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="G34">
+        <v>0.25</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0.25</v>
+      </c>
+      <c r="L34" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" s="2">
         <v>0.15</v>
       </c>
@@ -3416,8 +3695,20 @@
         <v>0</v>
       </c>
       <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="G35">
+        <v>0.25</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>0.25</v>
+      </c>
+      <c r="L35" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="2">
         <v>0.15</v>
       </c>
@@ -3431,8 +3722,20 @@
         <v>0</v>
       </c>
       <c r="E36" s="2"/>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="G36">
+        <v>0.25</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>0.25</v>
+      </c>
+      <c r="L36" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" s="2">
         <v>0.15</v>
       </c>
@@ -3446,8 +3749,17 @@
         <v>0</v>
       </c>
       <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>0.25</v>
+      </c>
+      <c r="L37" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" s="2">
         <v>0.15</v>
       </c>
@@ -3461,8 +3773,17 @@
         <v>0</v>
       </c>
       <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>0.25</v>
+      </c>
+      <c r="L38" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" s="2">
         <v>0.15</v>
       </c>
@@ -3476,8 +3797,21 @@
         <v>0</v>
       </c>
       <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <f>10/13*100</f>
+        <v>76.923076923076934</v>
+      </c>
+      <c r="K39">
+        <v>0.25</v>
+      </c>
+      <c r="L39" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" s="2">
         <v>0.15</v>
       </c>
@@ -3491,8 +3825,14 @@
         <v>0</v>
       </c>
       <c r="E40" s="2"/>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="K40">
+        <v>0.25</v>
+      </c>
+      <c r="L40" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" s="1">
         <v>0.15</v>
       </c>
@@ -3506,27 +3846,114 @@
         <v>0</v>
       </c>
       <c r="E41" s="2"/>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="K41">
+        <v>0.25</v>
+      </c>
+      <c r="L41" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="K42">
+        <v>0.25</v>
+      </c>
+      <c r="L42" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="K43">
+        <v>0.25</v>
+      </c>
+      <c r="L43" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
+      <c r="K44">
+        <v>0.25</v>
+      </c>
+      <c r="L44" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="K45">
+        <v>0.25</v>
+      </c>
+      <c r="L45" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="K46">
+        <v>0.25</v>
+      </c>
+      <c r="L46" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="K47">
+        <v>0.25</v>
+      </c>
+      <c r="L47" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="K48">
+        <v>0.25</v>
+      </c>
+      <c r="L48" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="11:13">
+      <c r="K49">
+        <v>0.25</v>
+      </c>
+      <c r="L49" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="11:13">
+      <c r="K50">
+        <v>0.25</v>
+      </c>
+      <c r="L50" s="4">
+        <v>1</v>
+      </c>
+      <c r="M50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="11:13">
+      <c r="K51">
+        <v>0.25</v>
+      </c>
+      <c r="L51" s="4">
+        <v>1</v>
+      </c>
+      <c r="M51">
+        <f>14/18*100</f>
+        <v>77.777777777777786</v>
+      </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="1"/>
@@ -3543,7 +3970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
@@ -4898,8 +5325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView topLeftCell="M10" workbookViewId="0">
-      <selection activeCell="T45" sqref="T45"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5622,13 +6049,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
+      <c r="B51" s="4"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
+      <c r="B52" s="4"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
@@ -5727,7 +6154,7 @@
   <dimension ref="B2:F10"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5776,7 +6203,7 @@
         <v>0.25</v>
       </c>
       <c r="C5">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E5">
         <v>90</v>
@@ -5790,7 +6217,7 @@
         <v>0.3</v>
       </c>
       <c r="C6">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D6">
         <v>0</v>

</xml_diff>